<commit_message>
checking in wash performance layouts and ap3 bom
</commit_message>
<xml_diff>
--- a/NI-2010/Lab Drawings/AP3/Drawings/AP3 DOE BOM.xlsx
+++ b/NI-2010/Lab Drawings/AP3/Drawings/AP3 DOE BOM.xlsx
@@ -5,24 +5,24 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Technology Lab\NI-2010\Lab Drawings\AP3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TechnologyLab\NI-2010\Lab Drawings\AP3\Drawings\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27800" windowHeight="12590"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="27804" windowHeight="12588"/>
   </bookViews>
   <sheets>
     <sheet name="Break Out" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Break Out'!$A$1:$H$16</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Break Out'!$A$1:$H$17</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="199">
   <si>
     <t>BILL OF MATERIALS</t>
   </si>
@@ -611,6 +611,15 @@
   </si>
   <si>
     <t>15V Power Supply</t>
+  </si>
+  <si>
+    <t>Camille Bauer</t>
+  </si>
+  <si>
+    <t>APLUS (Ethernet no display)</t>
+  </si>
+  <si>
+    <t>0112100</t>
   </si>
 </sst>
 </file>
@@ -655,7 +664,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -665,6 +674,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -696,7 +711,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -714,12 +729,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -734,15 +743,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -766,6 +766,47 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1107,232 +1148,224 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H63"/>
+  <dimension ref="A1:H64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C63" sqref="C63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="29" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.7265625" style="18" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.90625" style="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.54296875" style="18" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="75.54296875" style="19" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.81640625" style="18" customWidth="1"/>
-    <col min="7" max="7" width="19.81640625" style="18" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.81640625" style="18" customWidth="1"/>
-    <col min="9" max="9" width="8.7265625" style="1"/>
-    <col min="10" max="10" width="8.81640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="4.77734375" style="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.88671875" style="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.5546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="75.5546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.77734375" style="13" customWidth="1"/>
+    <col min="7" max="7" width="19.77734375" style="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.77734375" style="13" customWidth="1"/>
+    <col min="9" max="9" width="8.77734375" style="1"/>
+    <col min="10" max="10" width="8.77734375" style="1" customWidth="1"/>
     <col min="11" max="11" width="5" style="1" customWidth="1"/>
-    <col min="12" max="12" width="18.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="20.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="50.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="8.7265625" style="1"/>
+    <col min="12" max="12" width="18.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="50.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="8.77734375" style="1"/>
     <col min="19" max="19" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="4.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="16.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="4.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="16.21875" style="1" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="16" style="1" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="50" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="8.7265625" style="1"/>
-    <col min="25" max="25" width="9.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="8.77734375" style="1"/>
+    <col min="25" max="25" width="9.21875" style="1" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="8.7265625" style="1"/>
+    <col min="27" max="27" width="8.77734375" style="1"/>
     <col min="28" max="28" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="4.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="11.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="20.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="4.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="11.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="20.21875" style="1" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="49" style="1" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="7.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="5.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="8.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="36" max="16384" width="8.7265625" style="1"/>
+    <col min="33" max="33" width="7.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="5.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="8.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="36" max="16384" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
     </row>
     <row r="2" spans="1:8" ht="18.75" customHeight="1">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="21" t="s">
+      <c r="E2" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="H2" s="7" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="33" customHeight="1">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:8" ht="18.75" customHeight="1">
+      <c r="A3" s="21"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="31" t="s">
+        <v>198</v>
+      </c>
+      <c r="D3" s="21" t="s">
+        <v>196</v>
+      </c>
+      <c r="E3" s="22" t="s">
+        <v>197</v>
+      </c>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
+    </row>
+    <row r="4" spans="1:8" ht="33" customHeight="1">
+      <c r="A4" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B4" s="21">
         <v>1</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C4" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D4" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E4" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F4" s="24">
         <v>3175</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G4" s="24" t="s">
         <v>149</v>
       </c>
-      <c r="H3" s="5" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B4" s="2">
-        <v>1</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" s="5">
-        <v>202</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>155</v>
+      <c r="H4" s="24" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="2" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
       <c r="B5" s="2">
-        <v>3</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>189</v>
+        <v>1</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="22" t="s">
-        <v>188</v>
-      </c>
-      <c r="F5" s="10">
-        <v>15.25</v>
-      </c>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2" t="s">
-        <v>151</v>
+      <c r="E5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="5">
+        <v>202</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B6" s="2">
         <v>3</v>
       </c>
-      <c r="C6" s="11" t="s">
-        <v>186</v>
+      <c r="C6" s="9" t="s">
+        <v>189</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="23" t="s">
-        <v>187</v>
-      </c>
-      <c r="F6" s="10">
-        <v>550</v>
+      <c r="E6" s="17" t="s">
+        <v>188</v>
+      </c>
+      <c r="F6" s="8">
+        <v>15.25</v>
       </c>
       <c r="G6" s="2"/>
       <c r="H6" s="2" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="25.5" customHeight="1">
+    <row r="7" spans="1:8">
       <c r="A7" s="2" t="s">
-        <v>86</v>
+        <v>68</v>
       </c>
       <c r="B7" s="2">
         <v>3</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>71</v>
+      <c r="C7" s="9" t="s">
+        <v>186</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="F7" s="5">
-        <v>39</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="H7" s="5" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="12"/>
+      <c r="E7" s="18" t="s">
+        <v>187</v>
+      </c>
+      <c r="F7" s="8">
+        <v>550</v>
+      </c>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="25.5" customHeight="1">
+      <c r="A8" s="2" t="s">
+        <v>86</v>
+      </c>
       <c r="B8" s="2">
-        <v>1</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>105</v>
+        <v>3</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>71</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>106</v>
+        <v>72</v>
       </c>
       <c r="F8" s="5">
-        <v>315</v>
+        <v>39</v>
       </c>
       <c r="G8" s="5" t="s">
         <v>149</v>
@@ -1342,635 +1375,637 @@
       </c>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="2" t="s">
-        <v>114</v>
-      </c>
+      <c r="A9" s="10"/>
       <c r="B9" s="2">
-        <v>3</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>74</v>
+        <v>1</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>105</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="E9" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="F9" s="5">
+        <v>315</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" s="25" customFormat="1">
+      <c r="A10" s="21" t="s">
+        <v>114</v>
+      </c>
+      <c r="B10" s="21">
+        <v>3</v>
+      </c>
+      <c r="C10" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="D10" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="F9" s="10">
+      <c r="F10" s="23">
         <v>44.3</v>
       </c>
-      <c r="G9" s="2"/>
-      <c r="H9" s="5" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="A10" s="2" t="s">
+      <c r="G10" s="21"/>
+      <c r="H10" s="24" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B11" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C11" s="2" t="s">
         <v>84</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="F10" s="10">
-        <v>5.9</v>
-      </c>
-      <c r="G10" s="5">
-        <f>F10</f>
-        <v>5.9</v>
-      </c>
-      <c r="H10" s="5" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="21.75" customHeight="1">
-      <c r="A11" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>89</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="F11" s="10">
-        <v>39</v>
+        <v>83</v>
+      </c>
+      <c r="F11" s="8">
+        <v>5.9</v>
       </c>
       <c r="G11" s="5">
         <f>F11</f>
-        <v>39</v>
+        <v>5.9</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="21.75" customHeight="1">
       <c r="A12" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="B12" s="2">
-        <v>3</v>
+        <v>116</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E12" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="F12" s="8">
+        <v>39</v>
+      </c>
+      <c r="G12" s="5">
+        <f>F12</f>
+        <v>39</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" s="25" customFormat="1" ht="21.75" customHeight="1">
+      <c r="A13" s="21" t="s">
+        <v>117</v>
+      </c>
+      <c r="B13" s="21">
+        <v>3</v>
+      </c>
+      <c r="C13" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="D13" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="22" t="s">
         <v>88</v>
       </c>
-      <c r="F12" s="10">
+      <c r="F13" s="23">
         <v>2.4</v>
       </c>
-      <c r="G12" s="5">
-        <f>B12*F12</f>
+      <c r="G13" s="24">
+        <f>B13*F13</f>
         <v>7.1999999999999993</v>
       </c>
-      <c r="H12" s="5" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
-      <c r="A13" s="12"/>
-      <c r="B13" s="2">
+      <c r="H13" s="24" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="10"/>
+      <c r="B14" s="2">
         <v>3</v>
       </c>
-      <c r="C13" s="20" t="s">
+      <c r="C14" s="15" t="s">
         <v>185</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="E13" s="24" t="s">
-        <v>184</v>
-      </c>
-      <c r="F13" s="10">
-        <v>438.39</v>
-      </c>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8">
-      <c r="A14" s="12"/>
-      <c r="B14" s="2">
-        <v>5</v>
-      </c>
-      <c r="C14" s="2">
-        <v>105900</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="E14" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="F14" s="10">
-        <v>6.19</v>
-      </c>
-      <c r="G14" s="5">
-        <f>B14*F14</f>
-        <v>30.950000000000003</v>
-      </c>
+      <c r="E14" s="19" t="s">
+        <v>184</v>
+      </c>
+      <c r="F14" s="8">
+        <v>438.39</v>
+      </c>
+      <c r="G14" s="5"/>
       <c r="H14" s="5" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="12"/>
+      <c r="A15" s="10"/>
       <c r="B15" s="2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C15" s="2">
-        <v>108601</v>
+        <v>105900</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>92</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="F15" s="10">
-        <v>5.39</v>
+        <v>135</v>
+      </c>
+      <c r="F15" s="8">
+        <v>6.19</v>
       </c>
       <c r="G15" s="5">
         <f>B15*F15</f>
-        <v>5.39</v>
+        <v>30.950000000000003</v>
       </c>
       <c r="H15" s="5" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="12"/>
+      <c r="A16" s="10"/>
       <c r="B16" s="2">
-        <v>4</v>
-      </c>
-      <c r="C16" s="13">
-        <v>105902</v>
+        <v>1</v>
+      </c>
+      <c r="C16" s="2">
+        <v>108601</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>92</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="F16" s="10">
-        <v>10.59</v>
+        <v>134</v>
+      </c>
+      <c r="F16" s="8">
+        <v>5.39</v>
       </c>
       <c r="G16" s="5">
         <f>B16*F16</f>
-        <v>42.36</v>
+        <v>5.39</v>
       </c>
       <c r="H16" s="5" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="10"/>
+      <c r="B17" s="2">
+        <v>4</v>
+      </c>
+      <c r="C17" s="11">
+        <v>105902</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="F17" s="8">
+        <v>10.59</v>
+      </c>
+      <c r="G17" s="5">
+        <f>B17*F17</f>
+        <v>42.36</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" s="25" customFormat="1">
+      <c r="A18" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="B17" s="2">
+      <c r="B18" s="21">
         <v>1</v>
       </c>
-      <c r="C17" s="13" t="s">
+      <c r="C18" s="27" t="s">
         <v>191</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D18" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="E17" s="4" t="s">
+      <c r="E18" s="26" t="s">
         <v>192</v>
       </c>
-      <c r="F17" s="5">
+      <c r="F18" s="24">
         <v>390</v>
       </c>
-      <c r="G17" s="5" t="s">
+      <c r="G18" s="24" t="s">
         <v>149</v>
       </c>
-      <c r="H17" s="5" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8">
-      <c r="A18" s="2" t="s">
+      <c r="H18" s="24" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" s="25" customFormat="1">
+      <c r="A19" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B19" s="21">
         <v>1</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C19" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D19" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="E18" s="6" t="s">
+      <c r="E19" s="22" t="s">
         <v>82</v>
       </c>
-      <c r="F18" s="10">
+      <c r="F19" s="23">
         <v>1.91</v>
       </c>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8">
-      <c r="A19" s="2" t="s">
+      <c r="G19" s="24"/>
+      <c r="H19" s="24" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" s="25" customFormat="1">
+      <c r="A20" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="B19" s="14">
+      <c r="B20" s="28">
         <v>1</v>
       </c>
-      <c r="C19" s="13" t="s">
+      <c r="C20" s="27" t="s">
         <v>153</v>
       </c>
-      <c r="D19" s="14" t="s">
+      <c r="D20" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="E19" s="15" t="s">
+      <c r="E20" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="F19" s="16">
+      <c r="F20" s="30">
         <v>390</v>
       </c>
-      <c r="G19" s="5" t="s">
+      <c r="G20" s="24" t="s">
         <v>149</v>
       </c>
-      <c r="H19" s="5" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8">
-      <c r="A20" s="2" t="s">
+      <c r="H20" s="24" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" s="25" customFormat="1">
+      <c r="A21" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="B20" s="14">
+      <c r="B21" s="28">
         <v>1</v>
       </c>
-      <c r="C20" s="13" t="s">
+      <c r="C21" s="27" t="s">
         <v>154</v>
       </c>
-      <c r="D20" s="14" t="s">
+      <c r="D21" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="E20" s="15" t="s">
+      <c r="E21" s="29" t="s">
         <v>115</v>
       </c>
-      <c r="F20" s="16">
+      <c r="F21" s="30">
         <v>390</v>
       </c>
-      <c r="G20" s="5" t="s">
+      <c r="G21" s="24" t="s">
         <v>149</v>
       </c>
-      <c r="H20" s="5" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="15" customHeight="1">
-      <c r="A21" s="2" t="s">
+      <c r="H21" s="24" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" s="25" customFormat="1" ht="15" customHeight="1">
+      <c r="A22" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="B21" s="2">
+      <c r="B22" s="21">
         <v>1</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C22" s="21" t="s">
         <v>129</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="D22" s="21" t="s">
         <v>130</v>
       </c>
-      <c r="E21" s="4" t="s">
+      <c r="E22" s="26" t="s">
         <v>128</v>
       </c>
-      <c r="F21" s="5">
+      <c r="F22" s="24">
         <v>411</v>
       </c>
-      <c r="G21" s="5" t="s">
+      <c r="G22" s="24" t="s">
         <v>149</v>
       </c>
-      <c r="H21" s="5" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="15" customHeight="1">
-      <c r="A22" s="2"/>
-      <c r="B22" s="2">
+      <c r="H22" s="24" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="15" customHeight="1">
+      <c r="A23" s="21"/>
+      <c r="B23" s="21">
         <v>9</v>
       </c>
-      <c r="C22" s="11" t="s">
+      <c r="C23" s="32" t="s">
         <v>162</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="D23" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="E22" s="6" t="s">
+      <c r="E23" s="22" t="s">
         <v>163</v>
       </c>
-      <c r="F22" s="10">
+      <c r="F23" s="23">
         <v>22.97</v>
       </c>
-      <c r="G22" s="2"/>
-      <c r="H22" s="5" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8">
-      <c r="A23" s="2" t="s">
+      <c r="G23" s="21"/>
+      <c r="H23" s="24" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" s="21" t="s">
         <v>93</v>
       </c>
-      <c r="B23" s="2">
+      <c r="B24" s="21">
         <v>3</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C24" s="21" t="s">
         <v>98</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="D24" s="21" t="s">
         <v>97</v>
       </c>
-      <c r="E23" s="6" t="s">
+      <c r="E24" s="22" t="s">
         <v>99</v>
       </c>
-      <c r="F23" s="10">
+      <c r="F24" s="23">
         <v>6.13</v>
       </c>
-      <c r="G23" s="5"/>
-      <c r="H23" s="5" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="15" customHeight="1">
-      <c r="A24" s="2" t="s">
+      <c r="G24" s="24"/>
+      <c r="H24" s="24" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="15" customHeight="1">
+      <c r="A25" s="21" t="s">
         <v>94</v>
       </c>
-      <c r="B24" s="2">
+      <c r="B25" s="21">
         <v>3</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C25" s="21" t="s">
         <v>113</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="D25" s="21" t="s">
         <v>97</v>
       </c>
-      <c r="E24" s="6" t="s">
+      <c r="E25" s="22" t="s">
         <v>100</v>
       </c>
-      <c r="F24" s="10">
+      <c r="F25" s="23">
         <v>9.8000000000000007</v>
       </c>
-      <c r="G24" s="5"/>
-      <c r="H24" s="5" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8">
-      <c r="A25" s="2" t="s">
+      <c r="G25" s="24"/>
+      <c r="H25" s="24" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" s="21" t="s">
         <v>95</v>
       </c>
-      <c r="B25" s="2">
+      <c r="B26" s="21">
         <v>3</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C26" s="21" t="s">
         <v>101</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="D26" s="21" t="s">
         <v>97</v>
       </c>
-      <c r="E25" s="6" t="s">
+      <c r="E26" s="22" t="s">
         <v>103</v>
       </c>
-      <c r="F25" s="10">
+      <c r="F26" s="23">
         <v>7.61</v>
       </c>
-      <c r="G25" s="5"/>
-      <c r="H25" s="5" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8">
-      <c r="A26" s="2" t="s">
+      <c r="G26" s="24"/>
+      <c r="H26" s="24" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" s="21" t="s">
         <v>96</v>
       </c>
-      <c r="B26" s="2">
+      <c r="B27" s="21">
         <v>3</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C27" s="21" t="s">
         <v>102</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="D27" s="21" t="s">
         <v>97</v>
       </c>
-      <c r="E26" s="6" t="s">
+      <c r="E27" s="22" t="s">
         <v>104</v>
       </c>
-      <c r="F26" s="10">
+      <c r="F27" s="23">
         <v>13.01</v>
       </c>
-      <c r="G26" s="5"/>
-      <c r="H26" s="5" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8">
-      <c r="A27" s="2" t="s">
+      <c r="G27" s="24"/>
+      <c r="H27" s="24" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="B27" s="2">
+      <c r="B28" s="21">
         <v>1</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C28" s="21" t="s">
         <v>193</v>
       </c>
-      <c r="D27" s="3" t="s">
+      <c r="D28" s="33" t="s">
         <v>194</v>
       </c>
-      <c r="E27" s="4" t="s">
+      <c r="E28" s="26" t="s">
         <v>195</v>
       </c>
-      <c r="F27" s="5">
+      <c r="F28" s="24">
         <v>70.930000000000007</v>
       </c>
-      <c r="G27" s="2"/>
-      <c r="H27" s="5" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8">
-      <c r="A28" s="2" t="s">
+      <c r="G28" s="21"/>
+      <c r="H28" s="24" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" s="25" customFormat="1">
+      <c r="A29" s="21" t="s">
         <v>137</v>
       </c>
-      <c r="B28" s="2">
+      <c r="B29" s="21">
         <v>1</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C29" s="21" t="s">
         <v>142</v>
       </c>
-      <c r="D28" s="2" t="s">
+      <c r="D29" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="E28" s="6" t="s">
+      <c r="E29" s="22" t="s">
         <v>144</v>
       </c>
-      <c r="F28" s="10">
+      <c r="F29" s="23">
         <v>17.25</v>
       </c>
-      <c r="G28" s="5"/>
-      <c r="H28" s="5" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8">
-      <c r="A29" s="2" t="s">
+      <c r="G29" s="24"/>
+      <c r="H29" s="24" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" s="25" customFormat="1">
+      <c r="A30" s="21" t="s">
         <v>138</v>
       </c>
-      <c r="B29" s="2">
+      <c r="B30" s="21">
         <v>1</v>
       </c>
-      <c r="C29" s="7" t="s">
+      <c r="C30" s="31" t="s">
         <v>148</v>
       </c>
-      <c r="D29" s="2" t="s">
+      <c r="D30" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="E29" s="6" t="s">
+      <c r="E30" s="22" t="s">
         <v>145</v>
       </c>
-      <c r="F29" s="10">
+      <c r="F30" s="23">
         <v>2.1800000000000002</v>
       </c>
-      <c r="G29" s="5"/>
-      <c r="H29" s="5" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8">
-      <c r="A30" s="2" t="s">
+      <c r="G30" s="24"/>
+      <c r="H30" s="24" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" s="25" customFormat="1">
+      <c r="A31" s="21" t="s">
         <v>139</v>
       </c>
-      <c r="B30" s="2">
+      <c r="B31" s="21">
         <v>1</v>
       </c>
-      <c r="C30" s="2">
+      <c r="C31" s="21">
         <v>432000</v>
       </c>
-      <c r="D30" s="2" t="s">
+      <c r="D31" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="E30" s="6" t="s">
+      <c r="E31" s="22" t="s">
         <v>146</v>
       </c>
-      <c r="F30" s="10">
+      <c r="F31" s="23">
         <v>2.38</v>
       </c>
-      <c r="G30" s="5"/>
-      <c r="H30" s="5" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8">
-      <c r="A31" s="2" t="s">
+      <c r="G31" s="24"/>
+      <c r="H31" s="24" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" s="25" customFormat="1">
+      <c r="A32" s="21" t="s">
         <v>140</v>
       </c>
-      <c r="B31" s="2">
+      <c r="B32" s="21">
         <v>1</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="C32" s="21" t="s">
         <v>143</v>
       </c>
-      <c r="D31" s="2" t="s">
+      <c r="D32" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="E31" s="6" t="s">
+      <c r="E32" s="22" t="s">
         <v>147</v>
       </c>
-      <c r="F31" s="10">
+      <c r="F32" s="23">
         <v>4.99</v>
       </c>
-      <c r="G31" s="5"/>
-      <c r="H31" s="5" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8">
-      <c r="A32" s="2" t="s">
+      <c r="G32" s="24"/>
+      <c r="H32" s="24" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" s="25" customFormat="1">
+      <c r="A33" s="21" t="s">
         <v>141</v>
       </c>
-      <c r="B32" s="2">
+      <c r="B33" s="21">
         <v>1</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="C33" s="21" t="s">
         <v>160</v>
       </c>
-      <c r="D32" s="2" t="s">
+      <c r="D33" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="E32" s="6" t="s">
+      <c r="E33" s="22" t="s">
         <v>161</v>
       </c>
-      <c r="F32" s="10">
+      <c r="F33" s="23">
         <v>22.74</v>
       </c>
-      <c r="G32" s="5"/>
-      <c r="H32" s="5" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8">
-      <c r="A33" s="12"/>
-      <c r="B33" s="2">
+      <c r="G33" s="24"/>
+      <c r="H33" s="24" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="A34" s="10"/>
+      <c r="B34" s="2">
         <v>3</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="C34" s="2" t="s">
         <v>175</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="E33" s="6" t="s">
-        <v>176</v>
-      </c>
-      <c r="F33" s="10">
-        <v>450</v>
-      </c>
-      <c r="G33" s="2"/>
-      <c r="H33" s="5" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8">
-      <c r="A34" s="12"/>
-      <c r="B34" s="12">
-        <v>3</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>177</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>159</v>
       </c>
       <c r="E34" s="6" t="s">
-        <v>178</v>
-      </c>
-      <c r="F34" s="10">
-        <v>75.58</v>
+        <v>176</v>
+      </c>
+      <c r="F34" s="8">
+        <v>450</v>
       </c>
       <c r="G34" s="2"/>
       <c r="H34" s="5" t="s">
@@ -1978,21 +2013,21 @@
       </c>
     </row>
     <row r="35" spans="1:8">
-      <c r="A35" s="12"/>
-      <c r="B35" s="2">
+      <c r="A35" s="10"/>
+      <c r="B35" s="10">
         <v>3</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>159</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>180</v>
-      </c>
-      <c r="F35" s="10">
-        <v>134.47</v>
+        <v>178</v>
+      </c>
+      <c r="F35" s="8">
+        <v>75.58</v>
       </c>
       <c r="G35" s="2"/>
       <c r="H35" s="5" t="s">
@@ -2000,194 +2035,196 @@
       </c>
     </row>
     <row r="36" spans="1:8">
-      <c r="A36" s="2" t="s">
-        <v>46</v>
-      </c>
+      <c r="A36" s="10"/>
       <c r="B36" s="2">
         <v>3</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>7</v>
+        <v>179</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>159</v>
       </c>
       <c r="E36" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="F36" s="8">
+        <v>134.47</v>
+      </c>
+      <c r="G36" s="2"/>
+      <c r="H36" s="5" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" s="25" customFormat="1">
+      <c r="A37" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="B37" s="21">
+        <v>3</v>
+      </c>
+      <c r="C37" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="D37" s="21" t="s">
+        <v>159</v>
+      </c>
+      <c r="E37" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="F36" s="10">
+      <c r="F37" s="23">
         <v>2019</v>
       </c>
-      <c r="G36" s="5" t="s">
+      <c r="G37" s="24" t="s">
         <v>149</v>
       </c>
-      <c r="H36" s="5" t="s">
+      <c r="H37" s="24" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="37" spans="1:8">
-      <c r="A37" s="2" t="s">
+    <row r="38" spans="1:8" s="25" customFormat="1">
+      <c r="A38" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="B37" s="2">
+      <c r="B38" s="21">
         <v>3</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="C38" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="D37" s="2" t="s">
+      <c r="D38" s="21" t="s">
         <v>159</v>
       </c>
-      <c r="E37" s="6" t="s">
+      <c r="E38" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="F37" s="10">
+      <c r="F38" s="23">
         <v>536</v>
       </c>
-      <c r="G37" s="5" t="s">
+      <c r="G38" s="24" t="s">
         <v>149</v>
       </c>
-      <c r="H37" s="5" t="s">
+      <c r="H38" s="24" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="30" customHeight="1">
-      <c r="A38" s="2" t="s">
+    <row r="39" spans="1:8" s="25" customFormat="1" ht="30" customHeight="1">
+      <c r="A39" s="21" t="s">
         <v>124</v>
       </c>
-      <c r="B38" s="2">
+      <c r="B39" s="21">
         <v>1</v>
       </c>
-      <c r="C38" s="3" t="s">
+      <c r="C39" s="33" t="s">
         <v>125</v>
       </c>
-      <c r="D38" s="2" t="s">
+      <c r="D39" s="21" t="s">
         <v>126</v>
       </c>
-      <c r="E38" s="4" t="s">
+      <c r="E39" s="26" t="s">
         <v>127</v>
       </c>
-      <c r="F38" s="5">
+      <c r="F39" s="24">
         <v>478.99</v>
       </c>
-      <c r="G38" s="5" t="s">
+      <c r="G39" s="24" t="s">
         <v>149</v>
       </c>
-      <c r="H38" s="5" t="s">
+      <c r="H39" s="24" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="39" spans="1:8">
-      <c r="A39" s="2" t="s">
+    <row r="40" spans="1:8" s="25" customFormat="1">
+      <c r="A40" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="B39" s="2">
+      <c r="B40" s="21">
         <v>1</v>
       </c>
-      <c r="C39" s="2" t="s">
+      <c r="C40" s="21" t="s">
         <v>108</v>
       </c>
-      <c r="D39" s="2" t="s">
+      <c r="D40" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="E39" s="6" t="s">
+      <c r="E40" s="22" t="s">
         <v>107</v>
       </c>
-      <c r="F39" s="10">
+      <c r="F40" s="23">
         <v>461.4</v>
       </c>
-      <c r="G39" s="2"/>
-      <c r="H39" s="5" t="s">
+      <c r="G40" s="21"/>
+      <c r="H40" s="24" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="40" spans="1:8">
-      <c r="A40" s="2" t="s">
+    <row r="41" spans="1:8" s="25" customFormat="1">
+      <c r="A41" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="B40" s="2">
+      <c r="B41" s="21">
         <v>1</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="C41" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="D40" s="2" t="s">
+      <c r="D41" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="E40" s="6" t="s">
+      <c r="E41" s="22" t="s">
         <v>110</v>
       </c>
-      <c r="F40" s="10">
+      <c r="F41" s="23">
         <v>137.38</v>
       </c>
-      <c r="G40" s="2"/>
-      <c r="H40" s="5" t="s">
+      <c r="G41" s="21"/>
+      <c r="H41" s="24" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="41" spans="1:8">
-      <c r="A41" s="2" t="s">
+    <row r="42" spans="1:8" s="25" customFormat="1">
+      <c r="A42" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="B41" s="2">
+      <c r="B42" s="21">
         <v>2</v>
       </c>
-      <c r="C41" s="2" t="s">
+      <c r="C42" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="D41" s="2" t="s">
+      <c r="D42" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="E41" s="6" t="s">
+      <c r="E42" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="F41" s="10">
+      <c r="F42" s="23">
         <v>25.76</v>
       </c>
-      <c r="G41" s="2"/>
-      <c r="H41" s="5" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8">
-      <c r="A42" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B42" s="2">
-        <v>1</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E42" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="F42" s="10">
-        <v>2.5</v>
-      </c>
-      <c r="G42" s="2"/>
-      <c r="H42" s="5" t="s">
+      <c r="G42" s="21"/>
+      <c r="H42" s="24" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="43" spans="1:8">
       <c r="A43" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B43" s="2">
         <v>1</v>
       </c>
-      <c r="C43" s="2"/>
+      <c r="C43" s="2" t="s">
+        <v>35</v>
+      </c>
       <c r="D43" s="2" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="E43" s="6" t="s">
-        <v>157</v>
-      </c>
-      <c r="F43" s="10"/>
+        <v>26</v>
+      </c>
+      <c r="F43" s="8">
+        <v>2.5</v>
+      </c>
       <c r="G43" s="2"/>
       <c r="H43" s="5" t="s">
         <v>152</v>
@@ -2195,23 +2232,19 @@
     </row>
     <row r="44" spans="1:8">
       <c r="A44" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>41</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="B44" s="2">
+        <v>1</v>
+      </c>
+      <c r="C44" s="2"/>
       <c r="D44" s="2" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="E44" s="6" t="s">
-        <v>132</v>
-      </c>
-      <c r="F44" s="10">
-        <v>5.07</v>
-      </c>
+        <v>157</v>
+      </c>
+      <c r="F44" s="8"/>
       <c r="G44" s="2"/>
       <c r="H44" s="5" t="s">
         <v>152</v>
@@ -2219,22 +2252,22 @@
     </row>
     <row r="45" spans="1:8">
       <c r="A45" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="B45" s="2">
-        <v>1</v>
+        <v>59</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D45" s="2" t="s">
         <v>30</v>
       </c>
       <c r="E45" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="F45" s="10">
-        <v>5.94</v>
+        <v>132</v>
+      </c>
+      <c r="F45" s="8">
+        <v>5.07</v>
       </c>
       <c r="G45" s="2"/>
       <c r="H45" s="5" t="s">
@@ -2243,22 +2276,22 @@
     </row>
     <row r="46" spans="1:8">
       <c r="A46" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B46" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D46" s="2" t="s">
         <v>30</v>
       </c>
       <c r="E46" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="F46" s="10">
-        <v>1.04</v>
+        <v>21</v>
+      </c>
+      <c r="F46" s="8">
+        <v>5.94</v>
       </c>
       <c r="G46" s="2"/>
       <c r="H46" s="5" t="s">
@@ -2267,22 +2300,22 @@
     </row>
     <row r="47" spans="1:8">
       <c r="A47" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B47" s="2">
-        <v>41</v>
+        <v>2</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D47" s="2" t="s">
         <v>30</v>
       </c>
       <c r="E47" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F47" s="10">
-        <v>0.77</v>
+        <v>22</v>
+      </c>
+      <c r="F47" s="8">
+        <v>1.04</v>
       </c>
       <c r="G47" s="2"/>
       <c r="H47" s="5" t="s">
@@ -2291,22 +2324,22 @@
     </row>
     <row r="48" spans="1:8">
       <c r="A48" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B48" s="2">
-        <v>2</v>
+        <v>41</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>30</v>
       </c>
       <c r="E48" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="F48" s="2">
-        <v>0.53</v>
+        <v>23</v>
+      </c>
+      <c r="F48" s="8">
+        <v>0.77</v>
       </c>
       <c r="G48" s="2"/>
       <c r="H48" s="5" t="s">
@@ -2315,22 +2348,22 @@
     </row>
     <row r="49" spans="1:8">
       <c r="A49" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B49" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D49" s="2" t="s">
         <v>30</v>
       </c>
       <c r="E49" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="F49" s="10">
-        <v>0.34</v>
+        <v>24</v>
+      </c>
+      <c r="F49" s="2">
+        <v>0.53</v>
       </c>
       <c r="G49" s="2"/>
       <c r="H49" s="5" t="s">
@@ -2339,22 +2372,22 @@
     </row>
     <row r="50" spans="1:8">
       <c r="A50" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B50" s="2">
         <v>4</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>131</v>
+        <v>36</v>
       </c>
       <c r="D50" s="2" t="s">
         <v>30</v>
       </c>
       <c r="E50" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="F50" s="10">
-        <v>2.41</v>
+        <v>25</v>
+      </c>
+      <c r="F50" s="8">
+        <v>0.34</v>
       </c>
       <c r="G50" s="2"/>
       <c r="H50" s="5" t="s">
@@ -2363,22 +2396,22 @@
     </row>
     <row r="51" spans="1:8">
       <c r="A51" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B51" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>118</v>
+        <v>131</v>
       </c>
       <c r="D51" s="2" t="s">
         <v>30</v>
       </c>
       <c r="E51" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="F51" s="10">
-        <v>1.06</v>
+        <v>120</v>
+      </c>
+      <c r="F51" s="8">
+        <v>2.41</v>
       </c>
       <c r="G51" s="2"/>
       <c r="H51" s="5" t="s">
@@ -2387,86 +2420,86 @@
     </row>
     <row r="52" spans="1:8">
       <c r="A52" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="B52" s="2"/>
+        <v>66</v>
+      </c>
+      <c r="B52" s="2">
+        <v>2</v>
+      </c>
       <c r="C52" s="2" t="s">
-        <v>33</v>
+        <v>118</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E52" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="F52" s="10"/>
+        <v>119</v>
+      </c>
+      <c r="F52" s="8">
+        <v>1.06</v>
+      </c>
       <c r="G52" s="2"/>
       <c r="H52" s="5" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="53" spans="1:8">
-      <c r="A53" s="12"/>
-      <c r="B53" s="2">
+      <c r="A53" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B53" s="2"/>
+      <c r="C53" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E53" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F53" s="8"/>
+      <c r="G53" s="2"/>
+      <c r="H53" s="5" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8">
+      <c r="A54" s="10"/>
+      <c r="B54" s="2">
         <v>3</v>
       </c>
-      <c r="C53" s="2" t="s">
+      <c r="C54" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="D53" s="2" t="s">
+      <c r="D54" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="E53" s="6" t="s">
+      <c r="E54" s="6" t="s">
         <v>182</v>
       </c>
-      <c r="F53" s="10">
+      <c r="F54" s="8">
         <v>550</v>
       </c>
-      <c r="G53" s="2"/>
-      <c r="H53" s="2"/>
-    </row>
-    <row r="54" spans="1:8">
-      <c r="A54" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C54" s="2">
-        <v>1</v>
-      </c>
-      <c r="D54" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E54" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="F54" s="10">
-        <v>126.5</v>
-      </c>
       <c r="G54" s="2"/>
-      <c r="H54" s="5" t="s">
-        <v>158</v>
-      </c>
+      <c r="H54" s="2"/>
     </row>
     <row r="55" spans="1:8">
       <c r="A55" s="2" t="s">
-        <v>55</v>
+        <v>122</v>
       </c>
       <c r="B55" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C55" s="17" t="s">
-        <v>121</v>
+      <c r="C55" s="2">
+        <v>1</v>
       </c>
       <c r="D55" s="2" t="s">
         <v>44</v>
       </c>
       <c r="E55" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="F55" s="10">
-        <v>98</v>
+        <v>123</v>
+      </c>
+      <c r="F55" s="8">
+        <v>126.5</v>
       </c>
       <c r="G55" s="2"/>
       <c r="H55" s="5" t="s">
@@ -2475,22 +2508,22 @@
     </row>
     <row r="56" spans="1:8">
       <c r="A56" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="B56" s="2">
-        <v>2</v>
-      </c>
-      <c r="C56" s="2" t="s">
-        <v>31</v>
+        <v>55</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C56" s="12" t="s">
+        <v>121</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>11</v>
+        <v>44</v>
       </c>
       <c r="E56" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="F56" s="10">
-        <v>17</v>
+        <v>29</v>
+      </c>
+      <c r="F56" s="8">
+        <v>98</v>
       </c>
       <c r="G56" s="2"/>
       <c r="H56" s="5" t="s">
@@ -2499,113 +2532,115 @@
     </row>
     <row r="57" spans="1:8">
       <c r="A57" s="2" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="B57" s="2">
         <v>2</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>112</v>
+        <v>31</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>43</v>
+        <v>11</v>
       </c>
       <c r="E57" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="F57" s="10">
-        <v>4.43</v>
-      </c>
-      <c r="G57" s="5">
-        <f>B57*F57</f>
-        <v>8.86</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="F57" s="8">
+        <v>17</v>
+      </c>
+      <c r="G57" s="2"/>
       <c r="H57" s="5" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="58" spans="1:8">
-      <c r="A58" s="12"/>
+      <c r="A58" s="2" t="s">
+        <v>69</v>
+      </c>
       <c r="B58" s="2">
+        <v>2</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E58" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F58" s="8">
+        <v>4.43</v>
+      </c>
+      <c r="G58" s="5">
+        <f>B58*F58</f>
+        <v>8.86</v>
+      </c>
+      <c r="H58" s="5" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" s="25" customFormat="1">
+      <c r="A59" s="34"/>
+      <c r="B59" s="21">
         <v>15</v>
       </c>
-      <c r="C58" s="2" t="s">
+      <c r="C59" s="21" t="s">
         <v>166</v>
       </c>
-      <c r="D58" s="2" t="s">
+      <c r="D59" s="21" t="s">
         <v>167</v>
       </c>
-      <c r="E58" s="6" t="s">
+      <c r="E59" s="22" t="s">
         <v>169</v>
       </c>
-      <c r="F58" s="10">
+      <c r="F59" s="23">
         <v>26.82</v>
       </c>
-      <c r="G58" s="2"/>
-      <c r="H58" s="2" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8">
-      <c r="A59" s="12"/>
-      <c r="B59" s="2">
+      <c r="G59" s="21"/>
+      <c r="H59" s="21" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" s="25" customFormat="1">
+      <c r="A60" s="34"/>
+      <c r="B60" s="21">
         <v>15</v>
       </c>
-      <c r="C59" s="2" t="s">
+      <c r="C60" s="21" t="s">
         <v>170</v>
       </c>
-      <c r="D59" s="2" t="s">
+      <c r="D60" s="21" t="s">
         <v>167</v>
       </c>
-      <c r="E59" s="6" t="s">
+      <c r="E60" s="22" t="s">
         <v>168</v>
       </c>
-      <c r="F59" s="10">
+      <c r="F60" s="23">
         <v>14.25</v>
       </c>
-      <c r="G59" s="2"/>
-      <c r="H59" s="2" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8">
-      <c r="A60" s="12"/>
-      <c r="B60" s="2">
+      <c r="G60" s="21"/>
+      <c r="H60" s="21" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8">
+      <c r="A61" s="10"/>
+      <c r="B61" s="2">
         <v>9</v>
       </c>
-      <c r="C60" s="2" t="s">
+      <c r="C61" s="2" t="s">
         <v>171</v>
-      </c>
-      <c r="D60" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="E60" s="6" t="s">
-        <v>172</v>
-      </c>
-      <c r="F60" s="10">
-        <v>1.44</v>
-      </c>
-      <c r="G60" s="2"/>
-      <c r="H60" s="2" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8">
-      <c r="A61" s="12"/>
-      <c r="B61" s="2">
-        <v>3</v>
-      </c>
-      <c r="C61" s="2" t="s">
-        <v>173</v>
       </c>
       <c r="D61" s="2" t="s">
         <v>167</v>
       </c>
       <c r="E61" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="F61" s="10">
-        <v>35.729999999999997</v>
+        <v>172</v>
+      </c>
+      <c r="F61" s="8">
+        <v>1.44</v>
       </c>
       <c r="G61" s="2"/>
       <c r="H61" s="2" t="s">
@@ -2613,21 +2648,21 @@
       </c>
     </row>
     <row r="62" spans="1:8">
-      <c r="A62" s="12"/>
+      <c r="A62" s="10"/>
       <c r="B62" s="2">
         <v>3</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>164</v>
+        <v>173</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>44</v>
+        <v>167</v>
       </c>
       <c r="E62" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="F62" s="2">
-        <v>17.899999999999999</v>
+        <v>174</v>
+      </c>
+      <c r="F62" s="8">
+        <v>35.729999999999997</v>
       </c>
       <c r="G62" s="2"/>
       <c r="H62" s="2" t="s">
@@ -2635,29 +2670,51 @@
       </c>
     </row>
     <row r="63" spans="1:8">
-      <c r="A63" s="2" t="s">
+      <c r="A63" s="10"/>
+      <c r="B63" s="2">
+        <v>3</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E63" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="F63" s="2">
+        <v>17.899999999999999</v>
+      </c>
+      <c r="G63" s="2"/>
+      <c r="H63" s="2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8">
+      <c r="A64" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B63" s="2">
+      <c r="B64" s="2">
         <v>2</v>
       </c>
-      <c r="C63" s="2" t="s">
+      <c r="C64" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="D63" s="2" t="s">
+      <c r="D64" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E63" s="6" t="s">
+      <c r="E64" s="6" t="s">
         <v>183</v>
       </c>
-      <c r="F63" s="10">
+      <c r="F64" s="8">
         <v>4.43</v>
       </c>
-      <c r="G63" s="5">
-        <f>B63*F63</f>
+      <c r="G64" s="5">
+        <f>B64*F64</f>
         <v>8.86</v>
       </c>
-      <c r="H63" s="5" t="s">
+      <c r="H64" s="5" t="s">
         <v>158</v>
       </c>
     </row>

</xml_diff>